<commit_message>
Adição do crawler do Twitter
</commit_message>
<xml_diff>
--- a/Modelo.xlsx
+++ b/Modelo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Candidatos</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>Nome_Tematica</t>
-  </si>
-  <si>
-    <t>Link_Tweet</t>
   </si>
   <si>
     <t>Link_Noticia</t>
@@ -422,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,7 +466,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>12</v>
@@ -480,28 +477,17 @@
         <v>7</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E6" s="3" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E7" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Separando palavras e indexando-as
</commit_message>
<xml_diff>
--- a/Modelo.xlsx
+++ b/Modelo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Candidatos</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>Relevancia_Noticia</t>
+  </si>
+  <si>
+    <t>Quantidade_Tematica</t>
   </si>
 </sst>
 </file>
@@ -422,12 +425,13 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="18.7109375" customWidth="1"/>
+    <col min="1" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -479,10 +483,16 @@
       <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="G4" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E5" s="3" t="s">
         <v>13</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>